<commit_message>
Edited task status on scrum form
</commit_message>
<xml_diff>
--- a/Sudoku Game_Carter McCall_Personal/Low Expectations Scrum Project (Carter, Hosea, Isaiah).xlsx
+++ b/Sudoku Game_Carter McCall_Personal/Low Expectations Scrum Project (Carter, Hosea, Isaiah).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps_mu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d924908dd83d97b/Desktop/Classes/CSC1060/Unzipped/Sudoku Game_Carter McCall_Personal/Sudoku Game_Carter McCall_Personal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37D6DDFD-5BF2-429E-A05B-EC5A1EE90D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{37D6DDFD-5BF2-429E-A05B-EC5A1EE90D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC2DCF87-AF54-4C6A-AA08-DB4FEB8A4377}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="62">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>We decided to recreate the game, sudoku. Sudoku is a game played with numbers on a 9 x 9 grid. Each row and column must have numbers 1 through 9, used only once. There are also smaller squares made on a 3 x 3 grid. Each square must also have numbers 1 through 9. There must be no repeats and intersection in a row, column, or square. First, a board is printed a 9x9 the whole board is made and certain parts are hidden. Each board is randomized but has to follow the rules of sudoku. The most difficult part of the project is creating a check to make sure that each row, column, and square is having random numbers which have numbers 1 thorugh 9. An interesting part of the project is user interaction is making it into a grid and coordinate system. This makes the user select what want coordinate they want then input it. After seeing if their input is equal to the answer. If it is correct then the number would become visible. If it is not correct they would get to try again.</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -743,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4BDE91-026E-42C1-9643-D39E9BFB7C68}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -2436,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA0DA6C-A5EB-451E-A9B2-73656B28F8F2}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2585,7 +2588,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>13</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>10</v>
       </c>
@@ -2605,7 +2608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>Cover!B21</f>
         <v>All</v>
@@ -2619,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>Cover!B22</f>
         <v>All</v>
@@ -2633,7 +2636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>Cover!B23</f>
         <v>All</v>
@@ -2647,7 +2650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>52</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>41</v>
       </c>
@@ -2668,8 +2671,11 @@
       <c r="D25" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>44</v>
       </c>
@@ -2680,7 +2686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -2765,7 +2771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DDC301-48E9-474C-9B8D-1FA90964021A}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="102" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>

</xml_diff>